<commit_message>
Add SQL script to count employees managed by each manager using CTE and direct join methods
</commit_message>
<xml_diff>
--- a/Count_Employees/Problem_Statement.xlsx
+++ b/Count_Employees/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q13/Video_Q13_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Count_Employees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE43DFF-562A-7A48-BD6A-4CA6A492C051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB12D9C-C32E-4789-AEA5-EC486289C413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{EF528565-0254-9B49-BB74-2676380BA05E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{EF528565-0254-9B49-BB74-2676380BA05E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -99,29 +97,6 @@
   </si>
   <si>
     <t>NO_OF_EMPLOYEES</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Video #13 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Count Employees</t>
-    </r>
   </si>
   <si>
     <r>
@@ -144,6 +119,29 @@
       </rPr>
       <t xml:space="preserve">
 Find out the no of employees managed by each manager.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Count Employees</t>
     </r>
   </si>
 </sst>
@@ -456,15 +454,6 @@
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -498,17 +487,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,272 +843,272 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6ABE02-AF06-A941-866F-7BC16514FC73}">
   <dimension ref="C1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="18.83203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="7" width="10.796875" style="1"/>
+    <col min="8" max="8" width="18.796875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="C1" s="22" t="s">
+    <row r="1" spans="3:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="C1" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="3:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="3:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" spans="3:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="3:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="6" spans="3:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="3:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" spans="3:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" spans="3:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="6" spans="3:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="3:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="G7" s="2" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
+      <c r="G7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="3:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="3:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="10">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="7">
         <v>1</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="G9" s="10" t="s">
+      <c r="E9" s="9"/>
+      <c r="G9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="14">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="11">
         <v>2</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>1</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="14">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="11">
         <v>3</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>1</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="14">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="11">
         <v>4</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <v>1</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="14">
+    <row r="13" spans="3:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="11">
         <v>5</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="13">
         <v>2</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="14">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="11">
         <v>6</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="14">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="11">
         <v>7</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C16" s="14">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="11">
         <v>8</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C17" s="14">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="11">
         <v>9</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C18" s="14">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="11">
         <v>10</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C19" s="14">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="11">
         <v>11</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C20" s="14">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="11">
         <v>12</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="13">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C21" s="14">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="11">
         <v>13</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="13">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C22" s="14">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="11">
         <v>14</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="13">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="18">
+    <row r="23" spans="3:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="15">
         <v>15</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="18">
         <v>1</v>
       </c>
     </row>

</xml_diff>